<commit_message>
change some fields of certificates
</commit_message>
<xml_diff>
--- a/examples/excel_examples/course-credential.xlsx
+++ b/examples/excel_examples/course-credential.xlsx
@@ -299,7 +299,7 @@
     <t xml:space="preserve">user1@example.org</t>
   </si>
   <si>
-    <t xml:space="preserve">dni</t>
+    <t xml:space="preserve">18181818A</t>
   </si>
   <si>
     <t xml:space="preserve">online</t>
@@ -552,7 +552,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>